<commit_message>
moving to fyntrac-data repository
</commit_message>
<xml_diff>
--- a/model/processed_outputSO1.xlsx
+++ b/model/processed_outputSO1.xlsx
@@ -1721,7 +1721,7 @@
       <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n" s="81">
+      <c r="C2" t="n" s="77">
         <v>44712.0</v>
       </c>
       <c r="D2" t="s">
@@ -1730,13 +1730,13 @@
       <c r="E2" t="s">
         <v>104</v>
       </c>
-      <c r="F2" t="n" s="79">
+      <c r="F2" t="n" s="75">
         <v>1900.0</v>
       </c>
-      <c r="G2" t="n" s="82">
+      <c r="G2" t="n" s="78">
         <v>600.0</v>
       </c>
-      <c r="H2" t="n" s="80">
+      <c r="H2" t="n" s="76">
         <v>2500.0</v>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C4" t="n" s="77">
+      <c r="C4" t="n" s="81">
         <v>44712.0</v>
       </c>
       <c r="D4" t="s">
@@ -1782,13 +1782,13 @@
       <c r="E4" t="s">
         <v>104</v>
       </c>
-      <c r="F4" t="n" s="75">
+      <c r="F4" t="n" s="79">
         <v>1900.0</v>
       </c>
-      <c r="G4" t="n" s="78">
+      <c r="G4" t="n" s="82">
         <v>600.0</v>
       </c>
-      <c r="H4" s="76" t="n">
+      <c r="H4" s="80" t="n">
         <v>2500.0</v>
       </c>
     </row>

</xml_diff>